<commit_message>
updated readme and added scripts
</commit_message>
<xml_diff>
--- a/input_output_log.xlsx
+++ b/input_output_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22e7f93756eec4ea/vscode/ancestry_manuscript_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="558" documentId="11_F25DC773A252ABDACC1048CC091B69D25ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11D80EB-7BA8-45C3-96CD-23077D431F4C}"/>
+  <xr:revisionPtr revIDLastSave="597" documentId="11_F25DC773A252ABDACC1048CC091B69D25ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE044514-3D58-4B70-BA43-6F6549C33C26}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28200" yWindow="3492" windowWidth="23040" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="158">
   <si>
     <t>Notebook</t>
   </si>
@@ -183,9 +183,6 @@
     <t>avana_filtering_bed_file.bed</t>
   </si>
   <si>
-    <t>avana.filtered.ccle.variant.calls.vcf.gz</t>
-  </si>
-  <si>
     <t>snv_position_single_guide_finaldf.txt</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>./tcga_somatic/*avana.filtered</t>
   </si>
   <si>
-    <t>vcf_sample_sheet.tsv</t>
-  </si>
-  <si>
     <t>./tcga_germline/tcga_germline_sample_names.txt</t>
   </si>
   <si>
@@ -484,6 +478,27 @@
   </si>
   <si>
     <t>ccle.ancestry.snps.vcf.gz</t>
+  </si>
+  <si>
+    <t>./tcga_somatic/vcf_sample_sheet.tsv</t>
+  </si>
+  <si>
+    <t>create_affected_guides_per_gnomad_sample.R</t>
+  </si>
+  <si>
+    <t>final_randoms.txt</t>
+  </si>
+  <si>
+    <t>create_extracted_snps.R</t>
+  </si>
+  <si>
+    <t>top_snp_for_extraction.txt</t>
+  </si>
+  <si>
+    <t>create_top_snp_for_extraction.R</t>
+  </si>
+  <si>
+    <t>top.snp.fdr.txt</t>
   </si>
 </sst>
 </file>
@@ -545,6 +560,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -810,15 +829,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E171"/>
+  <dimension ref="A1:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" customWidth="1"/>
+    <col min="1" max="1" width="42.21875" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" customWidth="1"/>
     <col min="3" max="3" width="97.77734375" customWidth="1"/>
   </cols>
@@ -837,12 +856,12 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -851,7 +870,7 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -865,7 +884,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -879,7 +898,7 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -893,7 +912,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -907,7 +926,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -921,7 +940,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -935,7 +954,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -949,7 +968,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -963,7 +982,7 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -977,7 +996,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -991,12 +1010,12 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -1005,12 +1024,12 @@
         <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -1019,12 +1038,12 @@
         <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1033,12 +1052,12 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -1047,26 +1066,26 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -1075,12 +1094,12 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -1089,54 +1108,54 @@
         <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
         <v>112</v>
       </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>114</v>
-      </c>
       <c r="D20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
         <v>117</v>
       </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>119</v>
-      </c>
       <c r="D22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
@@ -1145,40 +1164,40 @@
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
@@ -1187,40 +1206,40 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
         <v>128</v>
       </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>130</v>
-      </c>
       <c r="D27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
@@ -1229,12 +1248,12 @@
         <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -1243,12 +1262,12 @@
         <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
@@ -1257,12 +1276,12 @@
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
@@ -1271,21 +1290,21 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1299,7 +1318,7 @@
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1310,10 +1329,10 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1327,7 +1346,7 @@
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1341,7 +1360,7 @@
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1355,7 +1374,7 @@
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1369,7 +1388,7 @@
         <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1383,7 +1402,7 @@
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1397,7 +1416,7 @@
         <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1411,7 +1430,7 @@
         <v>21</v>
       </c>
       <c r="D42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1425,7 +1444,7 @@
         <v>22</v>
       </c>
       <c r="D43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1439,7 +1458,7 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1453,7 +1472,7 @@
         <v>27</v>
       </c>
       <c r="D45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1467,7 +1486,7 @@
         <v>30</v>
       </c>
       <c r="D46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1481,7 +1500,7 @@
         <v>31</v>
       </c>
       <c r="D47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1495,7 +1514,7 @@
         <v>35</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1509,7 +1528,7 @@
         <v>36</v>
       </c>
       <c r="D49" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1523,7 +1542,7 @@
         <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1537,7 +1556,7 @@
         <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1551,7 +1570,7 @@
         <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1565,7 +1584,7 @@
         <v>51</v>
       </c>
       <c r="D53" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1576,10 +1595,10 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1590,584 +1609,584 @@
         <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D56" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D57" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D58" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D59" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D60" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D61" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
         <v>73</v>
       </c>
-      <c r="B62" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" t="s">
-        <v>75</v>
-      </c>
       <c r="D62" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D63" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D64" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D65" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D66" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D67" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D68" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B69" t="s">
         <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D69" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B70" t="s">
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D70" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D71" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
         <v>96</v>
       </c>
-      <c r="B72" t="s">
-        <v>6</v>
-      </c>
-      <c r="C72" t="s">
-        <v>98</v>
-      </c>
       <c r="D72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D73" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D76" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D77" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
         <v>107</v>
       </c>
-      <c r="B78" t="s">
-        <v>6</v>
-      </c>
-      <c r="C78" t="s">
-        <v>109</v>
-      </c>
       <c r="D78" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D79" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B80" t="s">
         <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D80" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D81" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D82" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B83" t="s">
         <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D83" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B84" t="s">
         <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D84" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B85" t="s">
         <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D85" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B86" t="s">
         <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D86" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>123</v>
+      </c>
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" t="s">
         <v>125</v>
       </c>
-      <c r="B87" t="s">
-        <v>6</v>
-      </c>
-      <c r="C87" t="s">
-        <v>127</v>
-      </c>
       <c r="D87" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B88" t="s">
         <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D88" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B89" t="s">
         <v>6</v>
       </c>
       <c r="C89" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D89" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B90" t="s">
         <v>6</v>
       </c>
       <c r="C90" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D90" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B91" t="s">
         <v>6</v>
       </c>
       <c r="C91" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D91" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B92" t="s">
         <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D92" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B93" t="s">
         <v>6</v>
       </c>
       <c r="C93" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D93" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B94" t="s">
         <v>6</v>
       </c>
       <c r="C94" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D94" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
+        <v>142</v>
+      </c>
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" t="s">
         <v>144</v>
       </c>
-      <c r="B95" t="s">
-        <v>6</v>
-      </c>
-      <c r="C95" t="s">
-        <v>146</v>
-      </c>
       <c r="D95" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
       </c>
       <c r="C96" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D96" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2181,7 +2200,7 @@
         <v>34</v>
       </c>
       <c r="D97" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -2195,7 +2214,7 @@
         <v>34</v>
       </c>
       <c r="D98" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -2209,7 +2228,7 @@
         <v>41</v>
       </c>
       <c r="D99" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2223,7 +2242,7 @@
         <v>42</v>
       </c>
       <c r="D100" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -2237,7 +2256,7 @@
         <v>43</v>
       </c>
       <c r="D101" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -2251,7 +2270,7 @@
         <v>46</v>
       </c>
       <c r="D102" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -2265,12 +2284,12 @@
         <v>29</v>
       </c>
       <c r="D103" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B104" t="s">
         <v>4</v>
@@ -2279,35 +2298,35 @@
         <v>29</v>
       </c>
       <c r="D104" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B105" t="s">
         <v>4</v>
       </c>
       <c r="C105" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D105" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B106" t="s">
         <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D106" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2321,7 +2340,7 @@
         <v>33</v>
       </c>
       <c r="D107" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -2335,7 +2354,7 @@
         <v>33</v>
       </c>
       <c r="D108" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2349,96 +2368,96 @@
         <v>33</v>
       </c>
       <c r="D109" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>55</v>
+      </c>
+      <c r="B110" t="s">
+        <v>4</v>
+      </c>
+      <c r="C110" t="s">
         <v>56</v>
       </c>
-      <c r="B110" t="s">
-        <v>4</v>
-      </c>
-      <c r="C110" t="s">
-        <v>57</v>
-      </c>
       <c r="D110" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B111" t="s">
         <v>4</v>
       </c>
       <c r="C111" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D111" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B112" t="s">
         <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D112" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B113" t="s">
         <v>4</v>
       </c>
       <c r="C113" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D113" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B114" t="s">
         <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D114" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B115" t="s">
         <v>4</v>
       </c>
       <c r="C115" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D115" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B116" t="s">
         <v>4</v>
@@ -2447,12 +2466,12 @@
         <v>33</v>
       </c>
       <c r="D116" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B117" t="s">
         <v>4</v>
@@ -2461,12 +2480,12 @@
         <v>33</v>
       </c>
       <c r="D117" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B118" t="s">
         <v>4</v>
@@ -2475,12 +2494,12 @@
         <v>33</v>
       </c>
       <c r="D118" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B119" t="s">
         <v>4</v>
@@ -2489,21 +2508,21 @@
         <v>33</v>
       </c>
       <c r="D119" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B120" t="s">
         <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D120" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -2517,7 +2536,7 @@
         <v>13</v>
       </c>
       <c r="D121" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -2531,7 +2550,7 @@
         <v>13</v>
       </c>
       <c r="D122" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -2545,12 +2564,12 @@
         <v>13</v>
       </c>
       <c r="D123" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B124" t="s">
         <v>4</v>
@@ -2559,21 +2578,21 @@
         <v>13</v>
       </c>
       <c r="D124" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B125" t="s">
         <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D125" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -2587,7 +2606,7 @@
         <v>38</v>
       </c>
       <c r="D126" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -2601,7 +2620,7 @@
         <v>45</v>
       </c>
       <c r="D127" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -2615,12 +2634,12 @@
         <v>45</v>
       </c>
       <c r="D128" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B129" t="s">
         <v>4</v>
@@ -2629,12 +2648,12 @@
         <v>45</v>
       </c>
       <c r="D129" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B130" t="s">
         <v>4</v>
@@ -2643,12 +2662,12 @@
         <v>45</v>
       </c>
       <c r="D130" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B131" t="s">
         <v>4</v>
@@ -2657,7 +2676,7 @@
         <v>45</v>
       </c>
       <c r="D131" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -2671,7 +2690,7 @@
         <v>5</v>
       </c>
       <c r="D132" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -2685,7 +2704,7 @@
         <v>12</v>
       </c>
       <c r="D133" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -2699,12 +2718,12 @@
         <v>12</v>
       </c>
       <c r="D134" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B135" t="s">
         <v>4</v>
@@ -2713,7 +2732,7 @@
         <v>12</v>
       </c>
       <c r="D135" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -2727,7 +2746,7 @@
         <v>24</v>
       </c>
       <c r="D136" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -2741,7 +2760,7 @@
         <v>24</v>
       </c>
       <c r="D137" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -2755,21 +2774,21 @@
         <v>24</v>
       </c>
       <c r="D138" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B139" t="s">
         <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D139" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
@@ -2783,7 +2802,7 @@
         <v>25</v>
       </c>
       <c r="D140" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -2794,10 +2813,10 @@
         <v>4</v>
       </c>
       <c r="C141" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D141" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -2811,7 +2830,7 @@
         <v>44</v>
       </c>
       <c r="D142" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
@@ -2824,318 +2843,405 @@
       <c r="C143" t="s">
         <v>47</v>
       </c>
+      <c r="D143" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>71</v>
+      </c>
+      <c r="B144" t="s">
+        <v>4</v>
+      </c>
+      <c r="C144" t="s">
+        <v>47</v>
+      </c>
+      <c r="D144" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>123</v>
+      </c>
+      <c r="B145" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" t="s">
+        <v>47</v>
+      </c>
+      <c r="D145" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>141</v>
+      </c>
+      <c r="B146" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" t="s">
+        <v>47</v>
+      </c>
+      <c r="D146" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>50</v>
       </c>
-      <c r="B144" t="s">
-        <v>4</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="B147" t="s">
+        <v>4</v>
+      </c>
+      <c r="C147" t="s">
+        <v>47</v>
+      </c>
+      <c r="D147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>50</v>
+      </c>
+      <c r="B148" t="s">
+        <v>4</v>
+      </c>
+      <c r="C148" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>50</v>
-      </c>
-      <c r="B145" t="s">
-        <v>4</v>
-      </c>
-      <c r="C145" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+      <c r="D148" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>64</v>
+      </c>
+      <c r="B149" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149" t="s">
+        <v>151</v>
+      </c>
+      <c r="D149" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>64</v>
+      </c>
+      <c r="B150" t="s">
+        <v>4</v>
+      </c>
+      <c r="C150" t="s">
         <v>65</v>
       </c>
-      <c r="B146" t="s">
-        <v>4</v>
-      </c>
-      <c r="C146" t="s">
+      <c r="D150" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>64</v>
+      </c>
+      <c r="B151" t="s">
+        <v>4</v>
+      </c>
+      <c r="C151" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>65</v>
-      </c>
-      <c r="B147" t="s">
-        <v>4</v>
-      </c>
-      <c r="C147" t="s">
+      <c r="D151" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>64</v>
+      </c>
+      <c r="B152" t="s">
+        <v>4</v>
+      </c>
+      <c r="C152" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>65</v>
-      </c>
-      <c r="B148" t="s">
-        <v>4</v>
-      </c>
-      <c r="C148" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>65</v>
-      </c>
-      <c r="B149" t="s">
-        <v>4</v>
-      </c>
-      <c r="C149" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>73</v>
-      </c>
-      <c r="B150" t="s">
-        <v>4</v>
-      </c>
-      <c r="C150" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>79</v>
-      </c>
-      <c r="B151" t="s">
-        <v>4</v>
-      </c>
-      <c r="C151" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>79</v>
-      </c>
-      <c r="B152" t="s">
-        <v>4</v>
-      </c>
-      <c r="C152" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D152" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B153" t="s">
         <v>4</v>
       </c>
       <c r="C153" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="D153" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B154" t="s">
         <v>4</v>
       </c>
       <c r="C154" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="D154" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="B155" t="s">
         <v>4</v>
       </c>
       <c r="C155" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="D155" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B156" t="s">
         <v>4</v>
       </c>
       <c r="C156" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+      <c r="D156" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="B157" t="s">
         <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="D157" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>79</v>
+        <v>154</v>
       </c>
       <c r="B158" t="s">
         <v>4</v>
       </c>
       <c r="C158" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+      <c r="D158" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>79</v>
+        <v>156</v>
       </c>
       <c r="B159" t="s">
         <v>4</v>
       </c>
       <c r="C159" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="D159" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="B160" t="s">
         <v>4</v>
       </c>
       <c r="C160" t="s">
-        <v>80</v>
+        <v>111</v>
+      </c>
+      <c r="D160" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B161" t="s">
         <v>4</v>
       </c>
       <c r="C161" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B162" t="s">
         <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="B163" t="s">
         <v>4</v>
       </c>
       <c r="C163" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="B164" t="s">
         <v>4</v>
       </c>
       <c r="C164" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="B165" t="s">
         <v>4</v>
       </c>
       <c r="C165" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="B166" t="s">
         <v>4</v>
       </c>
       <c r="C166" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="B167" t="s">
         <v>4</v>
       </c>
       <c r="C167" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="B168" t="s">
         <v>4</v>
       </c>
       <c r="C168" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="B169" t="s">
         <v>4</v>
       </c>
       <c r="C169" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B170" t="s">
         <v>4</v>
       </c>
       <c r="C170" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B171" t="s">
         <v>4</v>
       </c>
       <c r="C171" t="s">
-        <v>47</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>126</v>
+      </c>
+      <c r="B172" t="s">
+        <v>4</v>
+      </c>
+      <c r="C172" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>126</v>
+      </c>
+      <c r="B173" t="s">
+        <v>4</v>
+      </c>
+      <c r="C173" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>152</v>
+      </c>
+      <c r="B174" t="s">
+        <v>4</v>
+      </c>
+      <c r="C174" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E171">
-    <sortCondition ref="D2:D171"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E174">
+    <sortCondition ref="D2:D174"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>